<commit_message>
add total deaths plot
</commit_message>
<xml_diff>
--- a/www/data/Covid19.xlsx
+++ b/www/data/Covid19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selcukkorkmaz/Documents/GitHub/Covid2019Turkey/www/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4243449-FC23-484D-8D5F-2C6084FCC232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B71CD3C-25A0-8948-9126-9C4FFD4068EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1500" windowWidth="28300" windowHeight="17560" activeTab="2" xr2:uid="{25D0A33A-B1BF-C34E-B1E2-5CD2504B6A8B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Tarih</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Toplam Vaka/ Milyon Nüfus</t>
+  </si>
+  <si>
+    <t>Aktif Vaka</t>
   </si>
 </sst>
 </file>
@@ -1836,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C828EBED-D2FE-2A49-978F-915E70CFF528}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1942,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C12" si="0">B5-B4</f>
+        <f t="shared" ref="C5:C13" si="0">B5-B4</f>
         <v>0</v>
       </c>
       <c r="D5">
@@ -2104,6 +2107,28 @@
       </c>
       <c r="F12">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>43912</v>
+      </c>
+      <c r="B13">
+        <v>947</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>277</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <f>D13-D12</f>
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2113,18 +2138,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB03868D-6071-BD41-BDEC-20BB822B1411}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2132,39 +2157,46 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>670</v>
+        <v>947</v>
       </c>
       <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <f>A2-B2</f>
+        <v>926</v>
+      </c>
+      <c r="D2" s="6">
         <f>(B2/A2)*100</f>
-        <v>1.3432835820895521</v>
-      </c>
-      <c r="D2" s="5">
-        <f>1000000/F2</f>
-        <v>8.0572427896305499</v>
-      </c>
-      <c r="E2">
+        <v>2.2175290390707496</v>
+      </c>
+      <c r="E2" s="5">
+        <f>1000000/G2</f>
+        <v>11.388371525044972</v>
+      </c>
+      <c r="F2">
         <v>83154997</v>
       </c>
-      <c r="F2">
-        <f>E2/A2</f>
-        <v>124111.93582089552</v>
+      <c r="G2">
+        <f>F2/A2</f>
+        <v>87808.866948257652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>